<commit_message>
add: test for validation
</commit_message>
<xml_diff>
--- a/django_csv_test/book/tests/test_data/book.xlsx
+++ b/django_csv_test/book/tests/test_data/book.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Registered BY</t>
+          <t>Registered By</t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1862</t>
+          <t>6105</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -491,23 +491,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mean history clear six despite debate hear. Cut law second during born. Up role of difference.
-Father gas thing friend matter. Camera wife wait nothing long.</t>
+          <t>Quite main possible determine. Government capital later modern present.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:07</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:43</t>
+          <t>2022-11-26 14:48:07</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Atkins, Flores and Levy</t>
+          <t>Green, Martinez and Webb</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -534,7 +533,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4620</t>
+          <t>4830</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -544,22 +543,23 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>System quickly fly black individual including southern resource. Forward something that push avoid.</t>
+          <t>Pull myself model kid parent range point. Relationship why water subject above season agreement yet.
+Similar nation time news allow table.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:07</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:07</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Perkins-Herrera</t>
+          <t>Lawrence and Sons</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5126</t>
+          <t>4781</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -596,22 +596,23 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Too fear play. Outside apply girl yeah television spend analysis financial. Or wrong some direction play way prepare.</t>
+          <t>Wear behind far move successful. Arrive soldier training involve whom order.
+White open sure same between fact plan. Student fine yourself manage hour war amount.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:07</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Moran LLC</t>
+          <t>Schneider, Davenport and Mayer</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -638,33 +639,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>8657</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Remain red nearly happy threat onto. Wait government training little carry.
-Scene section suggest bar. Ever nice carry newspaper common myself. Marriage wife do practice.</t>
+          <t>War that which Congress expert person. Large she street five particular. Face senior officer mention ok physical not. Feeling wall create star fear couple.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Perez, Ritter and Rodgers</t>
+          <t>Gutierrez, Simmons and Moore</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6922</t>
+          <t>7855</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -701,23 +701,23 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Likely new rate operation public production. Too someone they late bad open.
-Notice drive all describe operation. Require offer another movie.</t>
+          <t>Friend thank research court remember owner skill.
+Way perhaps cause western probably sure. Start program safe should follow. But far account situation stay.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Singh PLC</t>
+          <t>Wolfe-Clayton</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3332</t>
+          <t>747</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -754,23 +754,23 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Face expect age task show less. Then several remain region sister particularly.
-Add lead could. Modern big east language.</t>
+          <t>Enter read important traditional interest believe gas. Knowledge scientist challenge partner mother since husband.
+Letter compare economy scene after. Question option pay standard friend safe.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Hardin and Sons</t>
+          <t>Anderson Group</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -797,7 +797,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9719</t>
+          <t>9588</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -807,22 +807,23 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Contain sense soldier director focus thought. Part tell teach office system north wear focus. Statement word enjoy whether of understand. Debate health grow huge table senior road statement.</t>
+          <t>Pattern bed action win approach which. President total wonder enter president rate.
+Others change owner like. Either catch fast fly this game hour drug. Represent relationship pay daughter.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Robertson Group</t>
+          <t>Chen Ltd</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -849,7 +850,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>493</t>
+          <t>9723</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -859,23 +860,22 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Mission lawyer recognize remain.
-Fill building effect if international. Usually much deal security admit.</t>
+          <t>Today across model politics just. Most concern I very. Particular industry wide stay.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Ponce, Conley and Golden</t>
+          <t>Montoya Group</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -902,7 +902,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4606</t>
+          <t>3487</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -912,23 +912,22 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>That data college serve use place without. Today ready order style drop deep move. War opportunity contain operation radio sometimes fine.
-Per anyone thank. Concern field accept employee great main.</t>
+          <t>Out kitchen knowledge recent. Let white difference woman exactly after wait. Small because rather statement meet. Though boy positive animal attack foreign.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:42</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>House, Thomas and Olsen</t>
+          <t>Kelly-Price</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -955,7 +954,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>9309</t>
+          <t>7577</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -965,22 +964,22 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Opportunity player threat former community seem within. Ball mouth today difference ready glass somebody. Detail support from stand hear together.</t>
+          <t>During sometimes news figure left garden. Today interesting face mouth. Recent yet thousand common every hold drive.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:06</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Mitchell-Garcia</t>
+          <t>Glover, George and Hill</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1007,7 +1006,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3351</t>
+          <t>8867</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1017,22 +1016,23 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Foreign expect century cut decade commercial tend. Growth administration candidate other. Current eye likely during property put wear.</t>
+          <t>Two job report final development beautiful media reason.
+Bar fund red today move military center true. Third it everybody think.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Carson Ltd</t>
+          <t>Davis-Sutton</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>7859</t>
+          <t>1528</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1069,23 +1069,23 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Town environment draw employee discussion finally rise. Cost us particularly professional place. Movie sign probably the.
-Receive party before. Current research administration here skin.</t>
+          <t>My direction simply tax main religious. Stop lawyer source network week together.
+Son value size positive project measure do. If election force war perform somebody. Require population same nor.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Taylor LLC</t>
+          <t>Lucero-Morrison</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2360</t>
+          <t>6394</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1122,23 +1122,23 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Food ready against let free power.
-Law within summer into edge value. Process information much mission piece. Popular particularly four effort play possible.</t>
+          <t>But ask bring ago old. Identify hold modern. Instead exactly actually name maybe form report.
+Detail a player man rule use large. Those successful foreign matter after. Leave another Republican.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Washington Ltd</t>
+          <t>Valencia-Hughes</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2163</t>
+          <t>9935</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1175,23 +1175,22 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Thus think cultural. Base baby believe.
-Figure remain individual person. Talk weight whom stop general. Father father difficult argue front. Executive product institution policy.</t>
+          <t>Billion meeting light agency. Leave after at and many theory. Pay eye indicate likely sell.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Bryant Group</t>
+          <t>Roberts-Michael</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1218,7 +1217,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5282</t>
+          <t>1357</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1228,23 +1227,23 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Part scene son research bring year from. Sign team marriage certain happen week three.
-Measure might player hair. Suffer be project party scientist too time.</t>
+          <t>Heart less one however show. Pressure strong administration their box deep factor. Action land effect look.
+Could suggest pretty laugh than. Society around have reveal speak white.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Carr-Thomas</t>
+          <t>Berger PLC</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1271,7 +1270,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>9264</t>
+          <t>2347</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1281,23 +1280,23 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Employee bank city economic million however. Natural break risk however. American oil good two.
-Everyone age during executive help well. Movement today land modern base during.</t>
+          <t>Increase well product purpose poor save.
+Possible analysis how author forward million. Try word three.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Jacobs, Maldonado and Adams</t>
+          <t>Lee PLC</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1324,7 +1323,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1799</t>
+          <t>4413</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1334,23 +1333,22 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Sit out number level ground magazine.
-Start bill hotel hard skill break almost. Itself water since edge color road threat determine.</t>
+          <t>Them trouble down here religious happen similar. May air machine radio near. Second before win teacher arrive through.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Petersen Inc</t>
+          <t>Duncan Group</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1377,7 +1375,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>8773</t>
+          <t>8136</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1387,22 +1385,23 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Worker produce seven attention wonder. Ball suggest across ball. Station really child detail thing catch.</t>
+          <t>Training plant population develop successful. Rule light hospital win win top type amount. Class follow computer car help.
+City may truth cover. Commercial church factor interest.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:41</t>
+          <t>2022-11-26 14:48:05</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Sullivan LLC</t>
+          <t>Young-Meyer</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1429,33 +1428,32 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>9401</t>
+          <t>1751</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Fear young adult perform pick what imagine those. Personal leave goal large six never third film. Follow least whether many administration class.
-Voice for remain Mrs. She up discuss.</t>
+          <t>Feeling class seat. Couple mouth behind line phone Mrs movie long. Environmental night information that office book car indicate.</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Strong, Tyler and Weaver</t>
+          <t>Robbins and Sons</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1482,7 +1480,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1673</t>
+          <t>8696</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1492,22 +1490,23 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Audience skin pull least. Really relationship no seek box threat summer.</t>
+          <t>Resource room shoulder product public. Put tell scene. Out everyone meeting. Majority lot by event.
+Civil lay return her campaign toward else. Step Republican Mrs might anything use.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Wells PLC</t>
+          <t>Brooks, Wong and Murphy</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1534,7 +1533,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>6930</t>
+          <t>8128</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1544,23 +1543,22 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Institution letter sound physical cold available. Certainly hospital guy part beat. Campaign interesting ready.
-Meet turn nor law could. Theory page writer message prove fill job.</t>
+          <t>None wonder debate Mr form since challenge. Instead several knowledge book weight visit. Send simple beautiful phone determine report.</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Myers, Green and Cortez</t>
+          <t>Huffman-Ortega</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1587,32 +1585,32 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>8777</t>
+          <t>4831</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Report option skin imagine address. See maintain quickly wife situation though pattern gun. Dinner history effort child left about it. Couple image race these.</t>
+          <t>Player type space term shake of western. Return either possible sense movement want.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Larsen Group</t>
+          <t>Andrade Ltd</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1639,32 +1637,33 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2088</t>
+          <t>4654</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Tonight development number rather direction program his market. Market decade serve picture measure. Citizen well serious interview.</t>
+          <t>Manage bag appear claim energy. Management dream thousand program something democratic eye.
+Life future deep discuss ask people available by. Then class wide major television middle.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Alvarado, Braun and Ross</t>
+          <t>Cruz, Matthews and Cox</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1691,33 +1690,33 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>6966</t>
+          <t>2308</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Hit Democrat wall ok economy ability evidence. Watch side interview candidate treat down student.
-Key head help partner usually. Expect cup policy certainly.</t>
+          <t>Color great program lawyer site inside owner read. Camera company since home far. Large television nor never start.
+Performance boy former need. Rock free box mother. Southern serious Mr sign.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Thompson-Shaffer</t>
+          <t>Smith PLC</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1744,33 +1743,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>9859</t>
+          <t>2964</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Could career care order. Least about hope something hope. Center process throughout record.
-Say political draw five pressure amount head. Charge sure drug return end. Natural enjoy agree else.</t>
+          <t>Six successful production product nearly. There individual foot former. People line before two east medical. Each course avoid on mention.</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:40</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Arroyo, Valdez and Chung</t>
+          <t>Hall Inc</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1797,7 +1795,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>9659</t>
+          <t>7939</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1807,23 +1805,23 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Group from generation. Tax generation official give mean above idea.
-While plan side investment magazine. Or how strategy line practice certainly from. Institution nice remember ball very pick quite.</t>
+          <t>Cultural suggest training leg. Move only rate stuff strategy.
+Very occur view resource. Both clearly our left to religious. Big because leader impact. However itself bed start same tell.</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:04</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Mosley-Nicholson</t>
+          <t>Paul, Ramirez and Scott</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1850,7 +1848,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3112</t>
+          <t>4471</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1860,23 +1858,22 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Late raise life rise edge. Soon suddenly nature room herself. Worker effort simply factor.
-Why financial high respond practice candidate rule. Create debate little full president music officer too.</t>
+          <t>Kitchen exactly discussion word something. Military outside growth individual whether suddenly method. Audience write feeling real relationship in.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Prince-Lozano</t>
+          <t>Bush, Chan and Hall</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1903,7 +1900,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>6656</t>
+          <t>7798</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1913,22 +1910,24 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Account property one growth police material. Fire according experience where service. Old among offer collection.</t>
+          <t>Available scientist radio baby box professor change.
+Lot contain yeah finish.
+Behind list participant question. New election future which both environment.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Hicks Group</t>
+          <t>Roberts-Cherry</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1955,7 +1954,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4432</t>
+          <t>1882</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1965,23 +1964,23 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Assume perform then turn investment sense. Their significant account. Significant camera water into decision least.
-Future paper international rest chance direction. Pm myself should to.</t>
+          <t>Campaign total couple meeting notice cut election western. Issue model me resource laugh happen crime.
+Represent sit for sign production environment anyone natural.</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Ramirez, Barber and Riley</t>
+          <t>Palmer-Greer</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2008,7 +2007,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1492</t>
+          <t>2562</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2018,22 +2017,24 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Simple situation chance that fall. Not second local home many else.</t>
+          <t>Meeting kid operation yet. Candidate our focus pretty card. Such body a fly place.
+Walk raise free future. High them memory house change.
+Kid sound me here.</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Boyle and Sons</t>
+          <t>Brewer Group</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2060,7 +2061,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7687</t>
+          <t>8398</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2070,24 +2071,23 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Her citizen ahead line west base. Interview major six tell.
-Any build south thousand fish safe. Edge partner wall page fire.
-Whose itself laugh now. Save seem recently some ability give.</t>
+          <t>Personal glass student day represent. Meeting oil same value Congress rock operation.
+Participant that state book. Full build technology stop. Respond about minute record nation dream arrive.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Padilla PLC</t>
+          <t>Bishop, Simmons and Hays</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4734</t>
+          <t>4393</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2124,23 +2124,22 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Total history instead performance director community. Mr know happen tree article rate talk. Dark century coach suggest.
-Single want garden partner view member.</t>
+          <t>Finish exist get civil name style energy. Board continue peace ago machine defense nice. Pressure room physical ability gun hospital.</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Jenkins, Callahan and Gross</t>
+          <t>Lopez-Miller</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2167,7 +2166,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>822</t>
+          <t>7190</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2177,23 +2176,22 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Also watch art close contain hundred. Clear board under standard year. Image safe hour religious. Against hot scene enough modern.
-Nice federal represent teach. Move but enough read.</t>
+          <t>Including pass sometimes go structure short. Large reveal once heart. Board offer wife structure protect job.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:39</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Gutierrez Ltd</t>
+          <t>Lozano, Brown and Smith</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2220,7 +2218,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>9854</t>
+          <t>6392</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2230,23 +2228,22 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Improve left tough network increase. Tree hard management bit source. Magazine prove unit itself reveal nation lead.
-Theory recent on beat. Shake and central owner direction decision.</t>
+          <t>Anyone must activity go. Production notice somebody hundred your smile. Attack late kind space foot. Example president character model avoid.</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:03</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Martin Ltd</t>
+          <t>Walker and Sons</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2273,7 +2270,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1040</t>
+          <t>9367</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2283,22 +2280,22 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Leg within when forget history arm week seem. Future outside enough level some town data. Try whether personal shoulder read of despite.</t>
+          <t>Center type public miss apply need value. Result side character. Watch center describe until computer study writer director.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Brown, Chapman and Knapp</t>
+          <t>Garcia, Lewis and Hunt</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2325,7 +2322,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7231</t>
+          <t>8571</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2335,23 +2332,23 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Blue benefit nice lawyer short. However skin up newspaper point dinner fast left.
-Physical production million art. Sound method Democrat full yet believe really.</t>
+          <t>Pressure put billion degree. Sound live report will suggest.
+Study turn others anyone offer operation up. But east break administration improve.</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Sexton and Sons</t>
+          <t>Turner-Lara</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2378,7 +2375,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1067</t>
+          <t>3300</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2388,22 +2385,23 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Building and many important cause party. Important opportunity ability accept.</t>
+          <t>Work back peace same artist certain machine not. Same son area stand quality.
+Prevent shoulder I something room rich possible. Per camera join. Memory kind staff body indeed those worry.</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Lopez LLC</t>
+          <t>Warren Group</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2430,7 +2428,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1791</t>
+          <t>7525</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2440,24 +2438,23 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Beat about provide. Crime single ok choice sign.
-Source choose science out.
-Single growth prepare trip summer. Bad itself girl week structure break.</t>
+          <t>Before continue bill their during record cut hair. Hot fast charge subject safe win.
+Her the middle close fund turn check. Against message treat world physical case break nearly.</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Hayes Inc</t>
+          <t>Anderson-Glover</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2484,7 +2481,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4337</t>
+          <t>9584</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2494,23 +2491,23 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Field apply significant huge drive early. Special Congress go.
-At discuss behavior goal special even bit. Law into well. Throughout specific conference low.</t>
+          <t>Current parent sell already down night sense. Executive let describe full avoid practice.
+Write environment himself good far race medical. Wrong since than church begin.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Hayden Inc</t>
+          <t>Martin and Sons</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2537,7 +2534,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7486</t>
+          <t>5052</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2547,23 +2544,23 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Truth campaign traditional draw per soldier water. Son admit author safe ability hit low. Nature pass center say.
-Health them quality. Among change seem wide summer class.</t>
+          <t>Sign big condition pretty understand fine beautiful.
+Defense ask imagine. View stop commercial some reason around.</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Miller-Carroll</t>
+          <t>Davis-Vincent</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2590,7 +2587,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8195</t>
+          <t>9975</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2600,23 +2597,22 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Guess table natural room team. Finally story your simple bed amount long.
-Available each such according benefit economy. Low million factor partner fear. Real certain wrong any cost require.</t>
+          <t>Speech already western hit sit rate. Political pretty should agency environment once near.</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Villanueva-Morton</t>
+          <t>Bowman-Mcneil</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2643,7 +2639,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5208</t>
+          <t>5596</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2653,22 +2649,22 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Stuff appear national face magazine. Successful lot economic until. Explain by point international detail because by.</t>
+          <t>Force bring environment nice treat couple. Suffer discussion even probably person whose. Should even card agency generation.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:38</t>
+          <t>2022-11-26 14:48:02</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Williams-Carlson</t>
+          <t>Phelps, Clark and Carr</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2695,7 +2691,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2491</t>
+          <t>3297</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2705,23 +2701,22 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Leave local like. Bag century sound make from.
-Continue member available window. Past right put team appear cup identify. Record section page behavior owner.</t>
+          <t>Cut capital success station speak activity. Take let word option marriage meeting general. Site soldier minute question shoulder continue.</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Jackson Inc</t>
+          <t>Wells-Johnson</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2748,33 +2743,33 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5119</t>
+          <t>8360</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Century same son off dark agree beat according. Physical television participant shoulder very.
-Story level ok safe.</t>
+          <t>Doctor know young million.
+Cause race have tell try several sometimes. Look house loss consider eye move smile society.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Reed-Morales</t>
+          <t>Camacho-Olson</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2801,33 +2796,32 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>8583</t>
+          <t>9595</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Image thank any book. Look language job performance see notice.
-Song special power question family long seem. School trade see television himself as.</t>
+          <t>Campaign artist board high soon sometimes. Sell section wonder meeting high read. Month walk surface successful. Resource result red although available political.</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Martin Inc</t>
+          <t>Benjamin-Sanchez</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2854,7 +2848,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6644</t>
+          <t>6166</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2864,22 +2858,23 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Season people image report knowledge nation special chance. Particular choice picture result while ball. Field all three experience person. Option compare property detail summer different.</t>
+          <t>Style every area adult responsibility. I people party information. Use long trip many child strong.
+Young light then close into relate. Attack its hard fall hundred father significant.</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Zimmerman, Thomas and Morris</t>
+          <t>Frazier Group</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2906,7 +2901,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2524</t>
+          <t>4732</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2916,23 +2911,24 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Teacher dog decade practice. Home brother health.
-Less clearly rise off bag. Standard both race everybody. Third receive after world after coach economic.</t>
+          <t>Candidate at form. Gas middle easy economy artist citizen sense capital.
+Huge financial cause. Without hair near.
+Property agree value way there. Certainly three focus majority.</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Foster Inc</t>
+          <t>Jones-Holloway</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2959,7 +2955,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5792</t>
+          <t>9519</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2969,23 +2965,23 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Break simply evidence option. Detail place sing artist ahead ago hair third. Investment special quite central process low trip.
-Various remain ok. Successful when cover kid.</t>
+          <t>Apply whether skin throw. Finish exactly such.
+Magazine own war. Discussion deep during speech.</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Miller, Schneider and Smith</t>
+          <t>Jacobs LLC</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3012,7 +3008,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7528</t>
+          <t>7382</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3022,23 +3018,24 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Rich view left few. Important care newspaper measure rock maintain raise.
-Spring past activity consumer box. Anything leave director hear difference short beat. Gun board media most.</t>
+          <t>Eight must close.
+Bad me however them husband. Consider party compare happy my. Especially each movement light.
+Evidence somebody worry fill could. Day tonight future certain you party.</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Williams Inc</t>
+          <t>Mathis, Knight and Williams</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3065,7 +3062,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>506</t>
+          <t>8056</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3075,23 +3072,22 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Effort issue impact fly. Letter partner opportunity must cup little.
-Win how compare individual think include. Window church team imagine foot doctor. Kind down glass late more beat.</t>
+          <t>We continue brother many. Their turn about budget we piece small. Staff word analysis parent middle art also.</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:00</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2022-11-04 22:37:37</t>
+          <t>2022-11-26 14:48:01</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Kramer, Wright and Duncan</t>
+          <t>Sullivan, Dixon and Salas</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">

</xml_diff>